<commit_message>
Changed micro symbol on template_FlowCal.xlsx
</commit_message>
<xml_diff>
--- a/examples/supporting_files/template_FlowCal.xlsx
+++ b/examples/supporting_files/template_FlowCal.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="1" r:id="rId1"/>
     <sheet name="Beads" sheetId="2" r:id="rId2"/>
     <sheet name="Samples" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" calcOnSave="0"/>
+  <calcPr calcId="171027" calcOnSave="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -99,16 +99,16 @@
     <t>FCFiles/Beads001.fcs</t>
   </si>
   <si>
-    <t>Flow PBS Volume (uL)</t>
-  </si>
-  <si>
-    <t>Flow Sample Volume (uL)</t>
+    <t>Flow Sample Volume (µL)</t>
+  </si>
+  <si>
+    <t>Flow PBS Volume (µL)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -488,7 +488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -551,7 +551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -621,11 +621,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,10 +657,10 @@
         <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>